<commit_message>
Day 4 - Arrays
</commit_message>
<xml_diff>
--- a/Problems Solved.xlsx
+++ b/Problems Solved.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="21">
   <si>
     <t>Problem</t>
   </si>
@@ -63,6 +63,30 @@
   </si>
   <si>
     <t>Prime Factors</t>
+  </si>
+  <si>
+    <t>All Divisors of a Number</t>
+  </si>
+  <si>
+    <t>Sieve of Erastosthenes</t>
+  </si>
+  <si>
+    <t>Arrays</t>
+  </si>
+  <si>
+    <t>Largest Element in Array</t>
+  </si>
+  <si>
+    <t>Second Largest</t>
+  </si>
+  <si>
+    <t>Check if array is sorted</t>
+  </si>
+  <si>
+    <t>Remove Duplicate elements from sorted array</t>
+  </si>
+  <si>
+    <t>Move all zeroes to end of array</t>
   </si>
 </sst>
 </file>
@@ -410,15 +434,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.109375" customWidth="1"/>
     <col min="2" max="2" width="38.6640625" customWidth="1"/>
-    <col min="3" max="3" width="35.77734375" customWidth="1"/>
+    <col min="3" max="3" width="39.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -535,49 +559,98 @@
       <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="C11" s="1"/>
+      <c r="B11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>11</v>
       </c>
+      <c r="B12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>12</v>
       </c>
+      <c r="B13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>13</v>
       </c>
+      <c r="B14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>14</v>
       </c>
+      <c r="B15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="1"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B19" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="1"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -592,8 +665,15 @@
     <hyperlink ref="C8" r:id="rId6"/>
     <hyperlink ref="C9" r:id="rId7"/>
     <hyperlink ref="C10" r:id="rId8"/>
+    <hyperlink ref="C11" r:id="rId9"/>
+    <hyperlink ref="C12" r:id="rId10"/>
+    <hyperlink ref="C13" r:id="rId11"/>
+    <hyperlink ref="C14" r:id="rId12"/>
+    <hyperlink ref="C15" r:id="rId13"/>
+    <hyperlink ref="C16" r:id="rId14"/>
+    <hyperlink ref="C17" r:id="rId15"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId16"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Day 5 - Arrays
</commit_message>
<xml_diff>
--- a/Problems Solved.xlsx
+++ b/Problems Solved.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="28">
   <si>
     <t>Problem</t>
   </si>
@@ -87,6 +87,27 @@
   </si>
   <si>
     <t>Move all zeroes to end of array</t>
+  </si>
+  <si>
+    <t>Difficulty Rating Order</t>
+  </si>
+  <si>
+    <t>Cost of Groceries</t>
+  </si>
+  <si>
+    <t>Running Comparison</t>
+  </si>
+  <si>
+    <t>Codechef Streak</t>
+  </si>
+  <si>
+    <t>Left Rotate an Array by One</t>
+  </si>
+  <si>
+    <t>Rotate Array by D Steps</t>
+  </si>
+  <si>
+    <t>Leader in an Array</t>
   </si>
 </sst>
 </file>
@@ -432,10 +453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -639,7 +660,9 @@
       <c r="B18" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="1"/>
+      <c r="C18" s="4" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
@@ -648,11 +671,107 @@
       <c r="B19" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="1"/>
+      <c r="C19" s="4" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>19</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>24</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="1"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
+        <v>25</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="1"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
+        <v>26</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" s="1"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
+        <v>27</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" s="1"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
+        <v>28</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -672,8 +791,15 @@
     <hyperlink ref="C15" r:id="rId13"/>
     <hyperlink ref="C16" r:id="rId14"/>
     <hyperlink ref="C17" r:id="rId15"/>
+    <hyperlink ref="C18" r:id="rId16"/>
+    <hyperlink ref="C19" r:id="rId17"/>
+    <hyperlink ref="C20" r:id="rId18"/>
+    <hyperlink ref="C21" r:id="rId19"/>
+    <hyperlink ref="C22" r:id="rId20"/>
+    <hyperlink ref="C23" r:id="rId21"/>
+    <hyperlink ref="C24" r:id="rId22"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId16"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId23"/>
 </worksheet>
 </file>
</xml_diff>